<commit_message>
DBMS Lerning Content Added
</commit_message>
<xml_diff>
--- a/Material.xlsx
+++ b/Material.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Android" sheetId="1" r:id="rId1"/>
     <sheet name="Git" sheetId="2" r:id="rId2"/>
-    <sheet name="Video Software" sheetId="3" r:id="rId3"/>
+    <sheet name="Useful Softwares and links" sheetId="3" r:id="rId3"/>
     <sheet name="Internship" sheetId="4" r:id="rId4"/>
+    <sheet name="DBMS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="250">
   <si>
     <t>https://developers.google.com/android/for-all/vocab-words/</t>
   </si>
@@ -554,6 +555,219 @@
   </si>
   <si>
     <t>framwork for developing apps in android, ios, windows, linux, etc.</t>
+  </si>
+  <si>
+    <t>Tuple</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>Domain or type</t>
+  </si>
+  <si>
+    <t>Each attribute will have type called string, text, jpg etc.</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>Structural description of relation in database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instance </t>
+  </si>
+  <si>
+    <t>Actual contents at given point in time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Null </t>
+  </si>
+  <si>
+    <t>Special value for unknown or undefined</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>attribute whose value is unique in each tuple or set of attributes whose combined values are unique</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>https://class.coursera.org/db/wiki/sql-guide</t>
+  </si>
+  <si>
+    <t>Quick Guide for MySQL, SQLite and PostgreSQL</t>
+  </si>
+  <si>
+    <t>https://class.coursera.org/db/wiki/xml-guide</t>
+  </si>
+  <si>
+    <t>Quickk guide for XML validation and querying</t>
+  </si>
+  <si>
+    <t>Quick Guide for RA relational algebra interpreter</t>
+  </si>
+  <si>
+    <t>https://class.coursera.org/db/wiki/ra-guide</t>
+  </si>
+  <si>
+    <t>http://www.nucleonsoftware.com/Products/Database-Master</t>
+  </si>
+  <si>
+    <t>Database Master Interface</t>
+  </si>
+  <si>
+    <t>http://www.tomjewett.com/dbdesign/dbdesign.php</t>
+  </si>
+  <si>
+    <t>Database design with UML and SQL</t>
+  </si>
+  <si>
+    <t>Distinct</t>
+  </si>
+  <si>
+    <t>Order by</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>table variables</t>
+  </si>
+  <si>
+    <t>set operators</t>
+  </si>
+  <si>
+    <t>union</t>
+  </si>
+  <si>
+    <t>intersaction</t>
+  </si>
+  <si>
+    <t>except</t>
+  </si>
+  <si>
+    <t>Where clause</t>
+  </si>
+  <si>
+    <t>join</t>
+  </si>
+  <si>
+    <t>condition1 and condition2</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>not in</t>
+  </si>
+  <si>
+    <t>exists</t>
+  </si>
+  <si>
+    <t>not exists</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>&lt;&gt;</t>
+  </si>
+  <si>
+    <t>not equal</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>abs</t>
+  </si>
+  <si>
+    <t>Subqueries in from</t>
+  </si>
+  <si>
+    <t>subqueries in select</t>
+  </si>
+  <si>
+    <t>Natural Join</t>
+  </si>
+  <si>
+    <t>Inner join on condition</t>
+  </si>
+  <si>
+    <t>Inner Join Using (attr)</t>
+  </si>
+  <si>
+    <t>Left|Right|Full outer join</t>
+  </si>
+  <si>
+    <t>Noinrmal Join</t>
+  </si>
+  <si>
+    <t>automatically join two table of same values</t>
+  </si>
+  <si>
+    <t>using</t>
+  </si>
+  <si>
+    <t>left outer join</t>
+  </si>
+  <si>
+    <t>natual left outer join</t>
+  </si>
+  <si>
+    <t>full outer join</t>
+  </si>
+  <si>
+    <t>right outer join</t>
+  </si>
+  <si>
+    <t>right natural outer join</t>
+  </si>
+  <si>
+    <t>Aggregation</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>Group by clause</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>having clause</t>
+  </si>
+  <si>
+    <t>is null</t>
+  </si>
+  <si>
+    <t>is not null</t>
+  </si>
+  <si>
+    <t>DDL</t>
+  </si>
+  <si>
+    <t>DML</t>
+  </si>
+  <si>
+    <t>insert</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>update</t>
   </si>
 </sst>
 </file>
@@ -606,7 +820,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -642,6 +856,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -650,7 +888,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -682,10 +920,23 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1182,10 +1433,10 @@
       </c>
     </row>
     <row r="25" spans="2:4" ht="48.75" customHeight="1">
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="15"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
@@ -1626,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1707,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1793,7 +2044,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>177</v>
       </c>
       <c r="B24" t="s">
@@ -1806,4 +2057,363 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:C62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15" customHeight="1">
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="30">
+      <c r="B17" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>218</v>
+      </c>
+      <c r="C23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="B33" s="17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="B34" s="17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="B35" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="19"/>
+      <c r="B37" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38" s="21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C39" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="B41" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="B42" s="21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="B43" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="B44" s="21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48" s="21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>